<commit_message>
Update Huntsville ELVI Survey.xlsx
</commit_message>
<xml_diff>
--- a/Summer Endophyte Surveys/Huntsville ELVI Survey.xlsx
+++ b/Summer Endophyte Surveys/Huntsville ELVI Survey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicampbell/Documents/GitHub/Fungal_Endophytes_Summer_2022/Summer Endophyte Surveys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66DF010-5D73-4A43-BB44-14B78DD7FD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4374CE2B-A379-1147-AC84-B15D5458F79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="17500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8609,9 +8609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81B5AFE-A0CF-F04E-B2E3-42B64BEC82CB}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:L51"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>